<commit_message>
r precision ok but not good results
</commit_message>
<xml_diff>
--- a/reports/results/metrics.xlsx
+++ b/reports/results/metrics.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\thesis-backup\thesis\reports\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C43E89-90FA-4B2A-806B-9DE264F92842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEEB2D3-CDE7-47A8-BDAA-873AA1790DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="precision" sheetId="1" r:id="rId1"/>
     <sheet name="recall" sheetId="3" r:id="rId2"/>
+    <sheet name="r_precision" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
   <si>
     <t>./models/bow_model.joblib</t>
   </si>
@@ -204,39 +205,68 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+  <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -274,35 +304,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -400,6 +401,39 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -527,6 +561,70 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -541,10 +639,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{527A628F-6082-4B41-B0C6-F9FC3AABFD09}" name="Table1" displayName="Table1" ref="A2:L11" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{527A628F-6082-4B41-B0C6-F9FC3AABFD09}" name="Table1" displayName="Table1" ref="A2:L11" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A2:L11" xr:uid="{527A628F-6082-4B41-B0C6-F9FC3AABFD09}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B7FAB6C4-0BD7-446B-9E90-BD6ED0B86E8B}" name="Column1" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{B7FAB6C4-0BD7-446B-9E90-BD6ED0B86E8B}" name="Column1" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{37799598-6971-4CB3-BF1F-2564F8D86D43}" name="./models/bow_model.joblib"/>
     <tableColumn id="3" xr3:uid="{41564B1F-33F3-448D-AFDC-35D65200896C}" name="./models/bigrams_bow_model.joblib"/>
     <tableColumn id="4" xr3:uid="{35EE790B-194C-41F7-BB80-A11858744BEB}" name="./models/trigrams_bow_model.joblib"/>
@@ -562,10 +660,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{735F3A25-5AF6-4539-9289-A66345A991AA}" name="Table2" displayName="Table2" ref="A15:L24" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{735F3A25-5AF6-4539-9289-A66345A991AA}" name="Table2" displayName="Table2" ref="A15:L24" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A15:L24" xr:uid="{735F3A25-5AF6-4539-9289-A66345A991AA}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{6C8F0A5F-8F55-476A-BFCF-BBAFB9910A6C}" name="Column1" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{6C8F0A5F-8F55-476A-BFCF-BBAFB9910A6C}" name="Column1" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{A3271BB2-DE77-4583-893E-74A7513B2B59}" name="./models/bow_model.joblib"/>
     <tableColumn id="3" xr3:uid="{7F4E68CC-D085-459B-BFCC-958FA6382DA6}" name="./models/bigrams_bow_model.joblib"/>
     <tableColumn id="4" xr3:uid="{67DCE8F0-8004-45F4-889C-61CF09974986}" name="./models/trigrams_bow_model.joblib"/>
@@ -583,42 +681,63 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{46DA7649-ED09-43D1-BC32-A8041C98B6CB}" name="Table3" displayName="Table3" ref="A2:L11" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{46DA7649-ED09-43D1-BC32-A8041C98B6CB}" name="Table3" displayName="Table3" ref="A2:L11" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A2:L11" xr:uid="{46DA7649-ED09-43D1-BC32-A8041C98B6CB}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{78FBF988-FD90-4D99-93B9-4F8A6CFA4BA6}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{38F554E8-9F0C-460B-8D1D-8020D9CF5534}" name="./models/bow_model.joblib" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{65B1EB45-6DC9-4626-A52D-5959123BB521}" name="./models/bigrams_bow_model.joblib" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{B60C90EF-DCCC-4633-9DE6-53FE857BC58C}" name="./models/trigrams_bow_model.joblib" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{57BCF9C0-756B-434D-9686-E74B1DD54483}" name="./models/tfidf_model.joblib" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{B042F7AF-3D54-4E94-85ED-D862C39BD7A5}" name="./models/bigrams_tfidf_model.joblib" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{EC1C01A0-9E35-470A-A911-2FDC6EDEFF1E}" name="./models/trigrams_tfidf_model.joblib" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{9687BD76-9638-4A10-834D-F30A955C0C13}" name="C:/Users/avitsas/Documents/VECTORS/word.w2v.200.bin" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{CC7689A5-522E-49FE-A825-66014A93F897}" name="C:/Users/avitsas/Documents/VECTORS/word.norm.w2v.200.bin" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{974A51C5-2EAC-420A-901C-D6916EBD904D}" name="word2vec-google-news-300" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{1B76D707-1B9B-4B64-B697-B43FD7BA92BF}" name="fasttext-wiki-news-subwords-300" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{AF6224D0-07C1-4F0D-BF72-646F50A8F736}" name="glove-twitter-200" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{78FBF988-FD90-4D99-93B9-4F8A6CFA4BA6}" name="Column1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{38F554E8-9F0C-460B-8D1D-8020D9CF5534}" name="./models/bow_model.joblib" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{65B1EB45-6DC9-4626-A52D-5959123BB521}" name="./models/bigrams_bow_model.joblib" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{B60C90EF-DCCC-4633-9DE6-53FE857BC58C}" name="./models/trigrams_bow_model.joblib" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{57BCF9C0-756B-434D-9686-E74B1DD54483}" name="./models/tfidf_model.joblib" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{B042F7AF-3D54-4E94-85ED-D862C39BD7A5}" name="./models/bigrams_tfidf_model.joblib" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{EC1C01A0-9E35-470A-A911-2FDC6EDEFF1E}" name="./models/trigrams_tfidf_model.joblib" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{9687BD76-9638-4A10-834D-F30A955C0C13}" name="C:/Users/avitsas/Documents/VECTORS/word.w2v.200.bin" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{CC7689A5-522E-49FE-A825-66014A93F897}" name="C:/Users/avitsas/Documents/VECTORS/word.norm.w2v.200.bin" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{974A51C5-2EAC-420A-901C-D6916EBD904D}" name="word2vec-google-news-300" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{1B76D707-1B9B-4B64-B697-B43FD7BA92BF}" name="fasttext-wiki-news-subwords-300" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{AF6224D0-07C1-4F0D-BF72-646F50A8F736}" name="glove-twitter-200" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D390A82F-5D5D-438F-B805-C9DE1B82447A}" name="Table4" displayName="Table4" ref="A15:L24" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D390A82F-5D5D-438F-B805-C9DE1B82447A}" name="Table4" displayName="Table4" ref="A15:L24" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A15:L24" xr:uid="{D390A82F-5D5D-438F-B805-C9DE1B82447A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B60A4E58-769F-4189-8B6C-133186E0157E}" name="Column1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3442BD1C-2E20-42FA-BC52-7FF9CE57918D}" name="./models/bow_model.joblib" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{76E40E9E-5B4D-4A00-9B74-80BFA1D56C39}" name="./models/bigrams_bow_model.joblib" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{726BAC1C-1416-428F-B0CE-4E4E6918DF33}" name="./models/trigrams_bow_model.joblib" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{2C306099-750E-4F5D-AC53-6E877AD0DF04}" name="./models/tfidf_model.joblib" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{1B76F280-FC0A-4D8E-869C-3261B08EE82E}" name="./models/bigrams_tfidf_model.joblib" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{664C044F-3DBC-4A1F-857D-AF408FE91B5A}" name="./models/trigrams_tfidf_model.joblib" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{EFB265EA-6FDF-4587-80E3-519FD2D1EF74}" name="C:/Users/avitsas/Documents/VECTORS/word.w2v.200.bin" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{69B22292-52BF-4C50-B3FF-0897737EDE08}" name="C:/Users/avitsas/Documents/VECTORS/word.norm.w2v.200.bin" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{5BFED889-0123-47F7-95D8-8FE0C0C9FC79}" name="word2vec-google-news-300" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{0CA15EC3-0087-4491-BFF8-E1C9E55FB33C}" name="fasttext-wiki-news-subwords-300" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{3DF125FD-301C-40C1-81B9-7C4CEBCEC8C6}" name="glove-twitter-200" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B60A4E58-769F-4189-8B6C-133186E0157E}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{3442BD1C-2E20-42FA-BC52-7FF9CE57918D}" name="./models/bow_model.joblib" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{76E40E9E-5B4D-4A00-9B74-80BFA1D56C39}" name="./models/bigrams_bow_model.joblib" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{726BAC1C-1416-428F-B0CE-4E4E6918DF33}" name="./models/trigrams_bow_model.joblib" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{2C306099-750E-4F5D-AC53-6E877AD0DF04}" name="./models/tfidf_model.joblib" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{1B76F280-FC0A-4D8E-869C-3261B08EE82E}" name="./models/bigrams_tfidf_model.joblib" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{664C044F-3DBC-4A1F-857D-AF408FE91B5A}" name="./models/trigrams_tfidf_model.joblib" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{EFB265EA-6FDF-4587-80E3-519FD2D1EF74}" name="C:/Users/avitsas/Documents/VECTORS/word.w2v.200.bin" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{69B22292-52BF-4C50-B3FF-0897737EDE08}" name="C:/Users/avitsas/Documents/VECTORS/word.norm.w2v.200.bin" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{5BFED889-0123-47F7-95D8-8FE0C0C9FC79}" name="word2vec-google-news-300" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{0CA15EC3-0087-4491-BFF8-E1C9E55FB33C}" name="fasttext-wiki-news-subwords-300" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{3DF125FD-301C-40C1-81B9-7C4CEBCEC8C6}" name="glove-twitter-200" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E557D1E5-E153-43CB-99C3-0A2484271D0E}" name="Table5" displayName="Table5" ref="A1:L10" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:L10" xr:uid="{E557D1E5-E153-43CB-99C3-0A2484271D0E}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3590CA5F-F581-45D4-B00F-03A772DDB471}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A6ED28F9-62EE-4032-ABFC-E41F632A4A2C}" name="./models/bow_model.joblib" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{573416F8-3184-45CB-A900-3D69D63F5D9C}" name="./models/bigrams_bow_model.joblib" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5E39EBAB-DFE0-45A5-ABC5-7CBE70D8207B}" name="./models/trigrams_bow_model.joblib" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{8DBCB55A-07BE-43EC-ABA7-0705B0DE4B62}" name="./models/tfidf_model.joblib" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{18599D46-685F-43A9-A85C-726B2D75B23D}" name="./models/bigrams_tfidf_model.joblib" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{C85083DD-2A21-406A-B9DF-60FC9B910D1A}" name="./models/trigrams_tfidf_model.joblib" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{7B54578B-C833-4E35-A755-825942F83620}" name="C:/Users/avitsas/Documents/VECTORS/word.w2v.200.bin" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{01F9A6BF-8AA4-4FE0-BEE5-F5E60BFEEE37}" name="C:/Users/avitsas/Documents/VECTORS/word.norm.w2v.200.bin" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{68E6A960-DA0A-497C-8A6F-917B2EE1F154}" name="word2vec-google-news-300" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{876C0555-7B1D-429F-B6E4-5C4D4908A3DF}" name="fasttext-wiki-news-subwords-300" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{FC981FE4-BC48-4865-9438-86683046E405}" name="glove-twitter-200" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1770,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CA628-A434-43F1-9F83-D4C0FE4812A1}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2598,4 +2717,417 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3BD529-2454-496B-88E6-04A183713980}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="7" max="7" width="35.44140625" customWidth="1"/>
+    <col min="8" max="8" width="52.21875" customWidth="1"/>
+    <col min="9" max="9" width="57.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="31.77734375" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>50</v>
+      </c>
+      <c r="I2" s="2">
+        <v>50</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>50</v>
+      </c>
+      <c r="K3" s="2">
+        <v>50</v>
+      </c>
+      <c r="L3" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2">
+        <v>50</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="D5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100</v>
+      </c>
+      <c r="F5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="G5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="H5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="I5" s="2">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="J5" s="2">
+        <v>50</v>
+      </c>
+      <c r="K5" s="2">
+        <v>50</v>
+      </c>
+      <c r="L5" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16.666666666666661</v>
+      </c>
+      <c r="E9" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="F9" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="G9" s="2">
+        <v>16.666666666666661</v>
+      </c>
+      <c r="H9" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="I9" s="2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2">
+        <v>25</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>